<commit_message>
templated files and progress report
Added folder for Templated Files and imported the spreadsheet showing
assets tied to entries up to 23 November prepared by jon johnson and
laura dosky
</commit_message>
<xml_diff>
--- a/Master List.xlsx
+++ b/Master List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12989" uniqueCount="5837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12990" uniqueCount="5838">
   <si>
     <t xml:space="preserve">Entry </t>
   </si>
@@ -17539,6 +17539,9 @@
   </si>
   <si>
     <t>Larionov, Mikhail</t>
+  </si>
+  <si>
+    <t>Cocoa Williams</t>
   </si>
 </sst>
 </file>
@@ -18878,8 +18881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4405" workbookViewId="0">
-      <selection activeCell="C4433" sqref="C4433"/>
+    <sheetView tabSelected="1" topLeftCell="A2135" workbookViewId="0">
+      <selection activeCell="B2150" sqref="B2150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -46697,7 +46700,9 @@
       <c r="A2154" s="60" t="s">
         <v>2722</v>
       </c>
-      <c r="B2154" s="61"/>
+      <c r="B2154" s="61" t="s">
+        <v>5837</v>
+      </c>
       <c r="C2154" s="61"/>
       <c r="D2154" s="62"/>
       <c r="E2154" s="60" t="s">

</xml_diff>